<commit_message>
added imported entities and hierarchy to import supersede file
</commit_message>
<xml_diff>
--- a/riscoss-webapp/src/main/webapp/resources/Supersede_IPR_Registry_v3.xlsx
+++ b/riscoss-webapp/src/main/webapp/resources/Supersede_IPR_Registry_v3.xlsx
@@ -58,40 +58,40 @@
     <t>Last update</t>
   </si>
   <si>
-    <t>WebContent</t>
+    <t>a1</t>
   </si>
   <si>
     <t>ASL3</t>
   </si>
   <si>
-    <t>itsdangerous 0.24</t>
+    <t>b1</t>
   </si>
   <si>
     <t>ASL2</t>
   </si>
   <si>
-    <t>typhoeus 0.7.1</t>
+    <t>c1</t>
   </si>
   <si>
     <t>Artistic2</t>
   </si>
   <si>
-    <t>Ganglia-web 3.6.2</t>
+    <t>d1</t>
   </si>
   <si>
     <t>LGPL2.1</t>
   </si>
   <si>
-    <t>RISCOSS</t>
-  </si>
-  <si>
-    <t>riscoss-data-collectors</t>
-  </si>
-  <si>
-    <t>riscoss-corporate</t>
-  </si>
-  <si>
-    <t>riscoss-analyser</t>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>d2</t>
   </si>
   <si>
     <t>License ID</t>
@@ -489,15 +489,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
+      <xdr:colOff>149040</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:rowOff>47520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>435960</xdr:colOff>
+      <xdr:colOff>462600</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>91080</xdr:rowOff>
+      <xdr:rowOff>81720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -512,8 +512,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="464760" y="56520"/>
-          <a:ext cx="2743560" cy="473040"/>
+          <a:off x="491760" y="47520"/>
+          <a:ext cx="2743200" cy="472680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -536,7 +536,7 @@
   <dimension ref="1:68"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75"/>

</xml_diff>